<commit_message>
Ajout des tests en échec M28 (UD sans document/fille) et M29 (cardinalité UD unique 0-1)
</commit_message>
<xml_diff>
--- a/Documentation/Developpement/Tableau_des_tests_effectues.xlsx
+++ b/Documentation/Developpement/Tableau_des_tests_effectues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Tests auto" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="294">
   <si>
     <t>Nom</t>
   </si>
@@ -887,6 +887,19 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>A renommer</t>
+  </si>
+  <si>
+    <t>M27_TestSansUniteDocumentaireErreur</t>
+  </si>
+  <si>
+    <t>On vérifie l'absence d'unité documentaire, ce qui rend donc une erreur</t>
+  </si>
+  <si>
+    <t>"\troot", ""
+"La présence d'une unité documentaire est obligatoire"</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1370,11 +1383,426 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="100">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1582,106 +2010,6 @@
         </vertical>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2135,206 +2463,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2711,46 +2839,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2876,30 +2964,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2911,78 +2975,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:F5002" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:F5002" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96">
   <tableColumns count="6">
-    <tableColumn id="1" name="Nom" dataDxfId="89"/>
-    <tableColumn id="2" name="Role" dataDxfId="88"/>
-    <tableColumn id="3" name="Resultat attendu" dataDxfId="87"/>
-    <tableColumn id="4" name="Resultat obtenu si echec" dataDxfId="86"/>
-    <tableColumn id="5" name="Modification a prevoir" dataDxfId="85"/>
-    <tableColumn id="6" name="Numéro d'ordre" dataDxfId="84"/>
+    <tableColumn id="1" name="Nom" dataDxfId="95"/>
+    <tableColumn id="2" name="Role" dataDxfId="94"/>
+    <tableColumn id="3" name="Resultat attendu" dataDxfId="93"/>
+    <tableColumn id="4" name="Resultat obtenu si echec" dataDxfId="92"/>
+    <tableColumn id="5" name="Modification a prevoir" dataDxfId="91"/>
+    <tableColumn id="6" name="Numéro d'ordre" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88" tableBorderDxfId="86" totalsRowBorderDxfId="85">
   <tableColumns count="11">
-    <tableColumn id="1" name="Profil testé" dataDxfId="74"/>
-    <tableColumn id="2" name="Nom tâche" dataDxfId="73"/>
-    <tableColumn id="3" name="Résultat test1" dataDxfId="72"/>
-    <tableColumn id="4" name="Si echec, stopper ici et écrire erreur test1" dataDxfId="71"/>
-    <tableColumn id="5" name="Résultat test2" dataDxfId="70"/>
-    <tableColumn id="6" name="Si echec, stopper ici et écrire erreur test2" dataDxfId="69"/>
-    <tableColumn id="7" name="Résultat test3" dataDxfId="68"/>
-    <tableColumn id="8" name="Si echec, stopper ici et écrire erreur test3" dataDxfId="67"/>
-    <tableColumn id="9" name="A revoir ?" dataDxfId="66"/>
-    <tableColumn id="10" name="Test à modifier" dataDxfId="65"/>
-    <tableColumn id="11" name="Phrase d'explication à mettre pour l'erreur" dataDxfId="64"/>
+    <tableColumn id="1" name="Profil testé" dataDxfId="84"/>
+    <tableColumn id="2" name="Nom tâche" dataDxfId="83"/>
+    <tableColumn id="3" name="Résultat test1" dataDxfId="82"/>
+    <tableColumn id="4" name="Si echec, stopper ici et écrire erreur test1" dataDxfId="81"/>
+    <tableColumn id="5" name="Résultat test2" dataDxfId="80"/>
+    <tableColumn id="6" name="Si echec, stopper ici et écrire erreur test2" dataDxfId="79"/>
+    <tableColumn id="7" name="Résultat test3" dataDxfId="78"/>
+    <tableColumn id="8" name="Si echec, stopper ici et écrire erreur test3" dataDxfId="77"/>
+    <tableColumn id="9" name="A revoir ?" dataDxfId="76"/>
+    <tableColumn id="10" name="Test à modifier" dataDxfId="75"/>
+    <tableColumn id="11" name="Phrase d'explication à mettre pour l'erreur" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:N1048576" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:N1048576" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70">
   <sortState ref="A2:N29">
     <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Balise strictement obligatoire" dataDxfId="39"/>
-    <tableColumn id="2" name="Nom en français" dataDxfId="38"/>
-    <tableColumn id="3" name="Version du SEDA" dataDxfId="37"/>
-    <tableColumn id="13" name="Chemin" dataDxfId="36"/>
-    <tableColumn id="4" name="Source auto, métier ou database" dataDxfId="35"/>
-    <tableColumn id="5" name="Créée lors de test ?" dataDxfId="34"/>
-    <tableColumn id="6" name="Balise falcultative" dataDxfId="33"/>
-    <tableColumn id="7" name="Nom en français2" dataDxfId="32"/>
-    <tableColumn id="8" name="Version" dataDxfId="31"/>
-    <tableColumn id="9" name="Chemin2" dataDxfId="30"/>
-    <tableColumn id="14" name="Source auto, métier ou database2" dataDxfId="29"/>
-    <tableColumn id="10" name="Quand obligatoire, créée lors de test ?" dataDxfId="28"/>
-    <tableColumn id="11" name="Quand falcultative, créée lors de test ?" dataDxfId="27"/>
-    <tableColumn id="12" name="Quand non-demandé, créée lors de test ?" dataDxfId="26"/>
+    <tableColumn id="1" name="Balise strictement obligatoire" dataDxfId="69"/>
+    <tableColumn id="2" name="Nom en français" dataDxfId="68"/>
+    <tableColumn id="3" name="Version du SEDA" dataDxfId="67"/>
+    <tableColumn id="13" name="Chemin" dataDxfId="66"/>
+    <tableColumn id="4" name="Source auto, métier ou database" dataDxfId="65"/>
+    <tableColumn id="5" name="Créée lors de test ?" dataDxfId="64"/>
+    <tableColumn id="6" name="Balise falcultative" dataDxfId="63"/>
+    <tableColumn id="7" name="Nom en français2" dataDxfId="62"/>
+    <tableColumn id="8" name="Version" dataDxfId="61"/>
+    <tableColumn id="9" name="Chemin2" dataDxfId="60"/>
+    <tableColumn id="14" name="Source auto, métier ou database2" dataDxfId="59"/>
+    <tableColumn id="10" name="Quand obligatoire, créée lors de test ?" dataDxfId="58"/>
+    <tableColumn id="11" name="Quand falcultative, créée lors de test ?" dataDxfId="57"/>
+    <tableColumn id="12" name="Quand non-demandé, créée lors de test ?" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A1:L1048576" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A1:L1048576" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52">
   <tableColumns count="12">
-    <tableColumn id="1" name="Attribut strictement obligatoire en v1.0" dataDxfId="11"/>
-    <tableColumn id="2" name="Nom en français" dataDxfId="10"/>
-    <tableColumn id="3" name="Version du SEDA" dataDxfId="9"/>
-    <tableColumn id="4" name="Chemin" dataDxfId="8"/>
-    <tableColumn id="5" name="Créée lors de test ?" dataDxfId="7"/>
-    <tableColumn id="6" name="Attribut falcultatif" dataDxfId="6"/>
-    <tableColumn id="7" name="Nom en français2" dataDxfId="5"/>
-    <tableColumn id="8" name="Version" dataDxfId="4"/>
-    <tableColumn id="9" name="Chemin2" dataDxfId="3"/>
-    <tableColumn id="10" name="Quand obligatoire, créée lors de test ?" dataDxfId="2"/>
-    <tableColumn id="11" name="Quand falcultatif, créée lors de test ?" dataDxfId="1"/>
-    <tableColumn id="12" name="Quand non-demandé, créé lors de test ?" dataDxfId="0"/>
+    <tableColumn id="1" name="Attribut strictement obligatoire en v1.0" dataDxfId="51"/>
+    <tableColumn id="2" name="Nom en français" dataDxfId="50"/>
+    <tableColumn id="3" name="Version du SEDA" dataDxfId="49"/>
+    <tableColumn id="4" name="Chemin" dataDxfId="48"/>
+    <tableColumn id="5" name="Créée lors de test ?" dataDxfId="47"/>
+    <tableColumn id="6" name="Attribut falcultatif" dataDxfId="46"/>
+    <tableColumn id="7" name="Nom en français2" dataDxfId="45"/>
+    <tableColumn id="8" name="Version" dataDxfId="44"/>
+    <tableColumn id="9" name="Chemin2" dataDxfId="43"/>
+    <tableColumn id="10" name="Quand obligatoire, créée lors de test ?" dataDxfId="42"/>
+    <tableColumn id="11" name="Quand falcultatif, créée lors de test ?" dataDxfId="41"/>
+    <tableColumn id="12" name="Quand non-demandé, créé lors de test ?" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3280,9 +3344,9 @@
   </sheetPr>
   <dimension ref="A1:F5002"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3315,7 +3379,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -3332,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -3350,7 +3414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -3368,7 +3432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -3386,7 +3450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>74</v>
       </c>
@@ -3404,7 +3468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>75</v>
       </c>
@@ -3422,7 +3486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="19" customFormat="1" ht="21" collapsed="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>118</v>
       </c>
@@ -3440,7 +3504,7 @@
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:6" s="21" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="21" customFormat="1" ht="38.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>76</v>
       </c>
@@ -3462,7 +3526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="21" customFormat="1" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="21" customFormat="1" ht="25.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>77</v>
       </c>
@@ -3482,7 +3546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>78</v>
       </c>
@@ -3504,7 +3568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>79</v>
       </c>
@@ -3526,7 +3590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>80</v>
       </c>
@@ -3548,7 +3612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>81</v>
       </c>
@@ -3570,7 +3634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="21" customFormat="1" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="21" customFormat="1" ht="25.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>82</v>
       </c>
@@ -3592,7 +3656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>83</v>
       </c>
@@ -3612,7 +3676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>84</v>
       </c>
@@ -3632,7 +3696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>85</v>
       </c>
@@ -3654,7 +3718,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>86</v>
       </c>
@@ -3674,7 +3738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="21" customFormat="1" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="21" customFormat="1" ht="25.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>87</v>
       </c>
@@ -3696,7 +3760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="21" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="21" customFormat="1" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>88</v>
       </c>
@@ -3716,7 +3780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="19" customFormat="1" ht="20.25" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>119</v>
       </c>
@@ -3768,11 +3832,11 @@
         <v>132</v>
       </c>
       <c r="E24" s="11" t="str">
-        <f t="shared" ref="E24:E49" si="3">IF(D24&lt;&gt;"Ok", "Oui", "Non")</f>
+        <f t="shared" ref="E24:E50" si="3">IF(D24&lt;&gt;"Ok", "Oui", "Non")</f>
         <v>Non</v>
       </c>
       <c r="F24" s="13">
-        <f t="shared" ref="F24:F49" si="4">F23+1</f>
+        <f t="shared" ref="F24:F48" si="4">F23+1</f>
         <v>21</v>
       </c>
     </row>
@@ -4293,54 +4357,59 @@
         <v>132</v>
       </c>
       <c r="E49" s="11" t="str">
+        <f t="shared" ref="E49" si="5">IF(D49&lt;&gt;"Ok", "Oui", "Non")</f>
+        <v>Non</v>
+      </c>
+      <c r="F49" s="13">
+        <f>F47+1</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" s="11" t="str">
         <f t="shared" si="3"/>
         <v>Non</v>
       </c>
-      <c r="F49" s="13">
-        <f t="shared" si="4"/>
+      <c r="F50" s="13">
+        <f>F48+1</f>
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="29" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
+    <row r="51" spans="1:6" s="29" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B50" s="25" t="s">
+      <c r="B51" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C50" s="25">
+      <c r="C51" s="25">
         <v>0</v>
       </c>
-      <c r="D50" s="26">
-        <f>COUNTIFS(E23:E49,"Oui")</f>
+      <c r="D51" s="26">
+        <f>COUNTIFS(E23:E50,"Oui")</f>
         <v>0</v>
       </c>
-      <c r="E50" s="27" t="str">
-        <f>IF(COUNTIF(E23:E49,"*Oui*")&lt;&gt;0, "Oui", "Non")</f>
+      <c r="E51" s="27" t="str">
+        <f>IF(COUNTIF(E23:E50,"*Oui*")&lt;&gt;0, "Oui", "Non")</f>
         <v>Non</v>
       </c>
-      <c r="F50" s="28"/>
-    </row>
-    <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F51" s="13">
-        <f>F49+1</f>
-        <v>47</v>
-      </c>
+      <c r="F51" s="28"/>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="12"/>
@@ -4351,13 +4420,13 @@
         <v>116</v>
       </c>
       <c r="F52" s="13">
-        <f>F51+1</f>
-        <v>48</v>
+        <f>F50+1</f>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
-        <v>10</v>
+      <c r="A53" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="12"/>
@@ -4368,13 +4437,13 @@
         <v>116</v>
       </c>
       <c r="F53" s="13">
-        <f t="shared" ref="F53:F116" si="5">F52+1</f>
-        <v>49</v>
+        <f>F52+1</f>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="12"/>
@@ -4385,13 +4454,13 @@
         <v>116</v>
       </c>
       <c r="F54" s="13">
-        <f t="shared" si="5"/>
-        <v>50</v>
+        <f t="shared" ref="F54:F117" si="6">F53+1</f>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="12"/>
@@ -4402,13 +4471,13 @@
         <v>116</v>
       </c>
       <c r="F55" s="13">
-        <f t="shared" si="5"/>
-        <v>51</v>
+        <f t="shared" si="6"/>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="12"/>
@@ -4419,13 +4488,13 @@
         <v>116</v>
       </c>
       <c r="F56" s="13">
-        <f t="shared" si="5"/>
-        <v>52</v>
+        <f t="shared" si="6"/>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="12"/>
@@ -4436,13 +4505,13 @@
         <v>116</v>
       </c>
       <c r="F57" s="13">
-        <f t="shared" si="5"/>
-        <v>53</v>
+        <f t="shared" si="6"/>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="12"/>
@@ -4453,13 +4522,13 @@
         <v>116</v>
       </c>
       <c r="F58" s="13">
-        <f t="shared" si="5"/>
-        <v>54</v>
+        <f t="shared" si="6"/>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="12"/>
@@ -4470,13 +4539,13 @@
         <v>116</v>
       </c>
       <c r="F59" s="13">
-        <f t="shared" si="5"/>
-        <v>55</v>
+        <f t="shared" si="6"/>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="12"/>
@@ -4487,13 +4556,13 @@
         <v>116</v>
       </c>
       <c r="F60" s="13">
-        <f t="shared" si="5"/>
-        <v>56</v>
+        <f t="shared" si="6"/>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B61" s="11"/>
       <c r="C61" s="12"/>
@@ -4504,13 +4573,13 @@
         <v>116</v>
       </c>
       <c r="F61" s="13">
-        <f t="shared" si="5"/>
-        <v>57</v>
+        <f t="shared" si="6"/>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="12"/>
@@ -4521,13 +4590,13 @@
         <v>116</v>
       </c>
       <c r="F62" s="13">
-        <f t="shared" si="5"/>
-        <v>58</v>
+        <f t="shared" si="6"/>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="12"/>
@@ -4538,13 +4607,13 @@
         <v>116</v>
       </c>
       <c r="F63" s="13">
-        <f t="shared" si="5"/>
-        <v>59</v>
+        <f t="shared" si="6"/>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="12"/>
@@ -4555,13 +4624,13 @@
         <v>116</v>
       </c>
       <c r="F64" s="13">
-        <f t="shared" si="5"/>
-        <v>60</v>
+        <f t="shared" si="6"/>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="12"/>
@@ -4572,13 +4641,13 @@
         <v>116</v>
       </c>
       <c r="F65" s="13">
-        <f t="shared" si="5"/>
-        <v>61</v>
+        <f t="shared" si="6"/>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="12"/>
@@ -4589,13 +4658,13 @@
         <v>116</v>
       </c>
       <c r="F66" s="13">
-        <f t="shared" si="5"/>
-        <v>62</v>
+        <f t="shared" si="6"/>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="12"/>
@@ -4606,13 +4675,13 @@
         <v>116</v>
       </c>
       <c r="F67" s="13">
-        <f t="shared" si="5"/>
-        <v>63</v>
+        <f t="shared" si="6"/>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B68" s="11"/>
       <c r="C68" s="12"/>
@@ -4623,13 +4692,13 @@
         <v>116</v>
       </c>
       <c r="F68" s="13">
-        <f t="shared" si="5"/>
-        <v>64</v>
+        <f t="shared" si="6"/>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="12"/>
@@ -4640,13 +4709,13 @@
         <v>116</v>
       </c>
       <c r="F69" s="13">
-        <f t="shared" si="5"/>
-        <v>65</v>
+        <f t="shared" si="6"/>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="12"/>
@@ -4657,13 +4726,13 @@
         <v>116</v>
       </c>
       <c r="F70" s="13">
-        <f t="shared" si="5"/>
-        <v>66</v>
+        <f t="shared" si="6"/>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B71" s="11"/>
       <c r="C71" s="12"/>
@@ -4674,13 +4743,13 @@
         <v>116</v>
       </c>
       <c r="F71" s="13">
-        <f t="shared" si="5"/>
-        <v>67</v>
+        <f t="shared" si="6"/>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B72" s="11"/>
       <c r="C72" s="12"/>
@@ -4691,13 +4760,13 @@
         <v>116</v>
       </c>
       <c r="F72" s="13">
-        <f t="shared" si="5"/>
-        <v>68</v>
+        <f t="shared" si="6"/>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="12"/>
@@ -4708,13 +4777,13 @@
         <v>116</v>
       </c>
       <c r="F73" s="13">
-        <f t="shared" si="5"/>
-        <v>69</v>
+        <f t="shared" si="6"/>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B74" s="11"/>
       <c r="C74" s="12"/>
@@ -4725,13 +4794,13 @@
         <v>116</v>
       </c>
       <c r="F74" s="13">
-        <f t="shared" si="5"/>
-        <v>70</v>
+        <f t="shared" si="6"/>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B75" s="11"/>
       <c r="C75" s="12"/>
@@ -4742,13 +4811,13 @@
         <v>116</v>
       </c>
       <c r="F75" s="13">
-        <f t="shared" si="5"/>
-        <v>71</v>
+        <f t="shared" si="6"/>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="12"/>
@@ -4759,13 +4828,13 @@
         <v>116</v>
       </c>
       <c r="F76" s="13">
-        <f t="shared" si="5"/>
-        <v>72</v>
+        <f t="shared" si="6"/>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B77" s="11"/>
       <c r="C77" s="12"/>
@@ -4776,13 +4845,13 @@
         <v>116</v>
       </c>
       <c r="F77" s="13">
-        <f t="shared" si="5"/>
-        <v>73</v>
+        <f t="shared" si="6"/>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B78" s="11"/>
       <c r="C78" s="12"/>
@@ -4793,13 +4862,13 @@
         <v>116</v>
       </c>
       <c r="F78" s="13">
-        <f t="shared" si="5"/>
-        <v>74</v>
+        <f t="shared" si="6"/>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B79" s="11"/>
       <c r="C79" s="12"/>
@@ -4810,13 +4879,13 @@
         <v>116</v>
       </c>
       <c r="F79" s="13">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="6"/>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B80" s="11"/>
       <c r="C80" s="12"/>
@@ -4827,13 +4896,13 @@
         <v>116</v>
       </c>
       <c r="F80" s="13">
-        <f t="shared" si="5"/>
-        <v>76</v>
+        <f t="shared" si="6"/>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B81" s="11"/>
       <c r="C81" s="12"/>
@@ -4844,13 +4913,13 @@
         <v>116</v>
       </c>
       <c r="F81" s="13">
-        <f t="shared" si="5"/>
-        <v>77</v>
+        <f t="shared" si="6"/>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B82" s="11"/>
       <c r="C82" s="12"/>
@@ -4861,13 +4930,13 @@
         <v>116</v>
       </c>
       <c r="F82" s="13">
-        <f t="shared" si="5"/>
-        <v>78</v>
+        <f t="shared" si="6"/>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B83" s="11"/>
       <c r="C83" s="12"/>
@@ -4878,13 +4947,13 @@
         <v>116</v>
       </c>
       <c r="F83" s="13">
-        <f t="shared" si="5"/>
-        <v>79</v>
+        <f t="shared" si="6"/>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="12"/>
@@ -4895,13 +4964,13 @@
         <v>116</v>
       </c>
       <c r="F84" s="13">
-        <f t="shared" si="5"/>
-        <v>80</v>
+        <f t="shared" si="6"/>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="12"/>
@@ -4912,13 +4981,13 @@
         <v>116</v>
       </c>
       <c r="F85" s="13">
-        <f t="shared" si="5"/>
-        <v>81</v>
+        <f t="shared" si="6"/>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B86" s="11"/>
       <c r="C86" s="12"/>
@@ -4929,13 +4998,13 @@
         <v>116</v>
       </c>
       <c r="F86" s="13">
-        <f t="shared" si="5"/>
-        <v>82</v>
+        <f t="shared" si="6"/>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B87" s="11"/>
       <c r="C87" s="12"/>
@@ -4946,13 +5015,13 @@
         <v>116</v>
       </c>
       <c r="F87" s="13">
-        <f t="shared" si="5"/>
-        <v>83</v>
+        <f t="shared" si="6"/>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B88" s="11"/>
       <c r="C88" s="12"/>
@@ -4963,13 +5032,13 @@
         <v>116</v>
       </c>
       <c r="F88" s="13">
-        <f t="shared" si="5"/>
-        <v>84</v>
+        <f t="shared" si="6"/>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B89" s="11"/>
       <c r="C89" s="12"/>
@@ -4980,13 +5049,13 @@
         <v>116</v>
       </c>
       <c r="F89" s="13">
-        <f t="shared" si="5"/>
-        <v>85</v>
+        <f t="shared" si="6"/>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B90" s="11"/>
       <c r="C90" s="12"/>
@@ -4997,13 +5066,13 @@
         <v>116</v>
       </c>
       <c r="F90" s="13">
-        <f t="shared" si="5"/>
-        <v>86</v>
+        <f t="shared" si="6"/>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" s="11"/>
       <c r="C91" s="12"/>
@@ -5014,13 +5083,13 @@
         <v>116</v>
       </c>
       <c r="F91" s="13">
-        <f t="shared" si="5"/>
-        <v>87</v>
+        <f t="shared" si="6"/>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="12"/>
@@ -5031,13 +5100,13 @@
         <v>116</v>
       </c>
       <c r="F92" s="13">
-        <f t="shared" si="5"/>
-        <v>88</v>
+        <f t="shared" si="6"/>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="12"/>
@@ -5048,13 +5117,13 @@
         <v>116</v>
       </c>
       <c r="F93" s="13">
-        <f t="shared" si="5"/>
-        <v>89</v>
+        <f t="shared" si="6"/>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B94" s="11"/>
       <c r="C94" s="12"/>
@@ -5065,13 +5134,13 @@
         <v>116</v>
       </c>
       <c r="F94" s="13">
-        <f t="shared" si="5"/>
-        <v>90</v>
+        <f t="shared" si="6"/>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B95" s="11"/>
       <c r="C95" s="12"/>
@@ -5082,13 +5151,13 @@
         <v>116</v>
       </c>
       <c r="F95" s="13">
-        <f t="shared" si="5"/>
-        <v>91</v>
+        <f t="shared" si="6"/>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B96" s="11"/>
       <c r="C96" s="12"/>
@@ -5099,13 +5168,13 @@
         <v>116</v>
       </c>
       <c r="F96" s="13">
-        <f t="shared" si="5"/>
-        <v>92</v>
+        <f t="shared" si="6"/>
+        <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B97" s="11"/>
       <c r="C97" s="12"/>
@@ -5116,13 +5185,13 @@
         <v>116</v>
       </c>
       <c r="F97" s="13">
-        <f t="shared" si="5"/>
-        <v>93</v>
+        <f t="shared" si="6"/>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="12"/>
@@ -5133,13 +5202,13 @@
         <v>116</v>
       </c>
       <c r="F98" s="13">
-        <f t="shared" si="5"/>
-        <v>94</v>
+        <f t="shared" si="6"/>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B99" s="11"/>
       <c r="C99" s="12"/>
@@ -5150,13 +5219,13 @@
         <v>116</v>
       </c>
       <c r="F99" s="13">
-        <f t="shared" si="5"/>
-        <v>95</v>
+        <f t="shared" si="6"/>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B100" s="11"/>
       <c r="C100" s="12"/>
@@ -5167,13 +5236,13 @@
         <v>116</v>
       </c>
       <c r="F100" s="13">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="6"/>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B101" s="11"/>
       <c r="C101" s="12"/>
@@ -5184,13 +5253,13 @@
         <v>116</v>
       </c>
       <c r="F101" s="13">
-        <f t="shared" si="5"/>
-        <v>97</v>
+        <f t="shared" si="6"/>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B102" s="11"/>
       <c r="C102" s="12"/>
@@ -5201,13 +5270,13 @@
         <v>116</v>
       </c>
       <c r="F102" s="13">
-        <f t="shared" si="5"/>
-        <v>98</v>
+        <f t="shared" si="6"/>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B103" s="11"/>
       <c r="C103" s="12"/>
@@ -5218,13 +5287,13 @@
         <v>116</v>
       </c>
       <c r="F103" s="13">
-        <f t="shared" si="5"/>
-        <v>99</v>
+        <f t="shared" si="6"/>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B104" s="11"/>
       <c r="C104" s="12"/>
@@ -5235,13 +5304,13 @@
         <v>116</v>
       </c>
       <c r="F104" s="13">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <f t="shared" si="6"/>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B105" s="11"/>
       <c r="C105" s="12"/>
@@ -5252,13 +5321,13 @@
         <v>116</v>
       </c>
       <c r="F105" s="13">
-        <f t="shared" si="5"/>
-        <v>101</v>
+        <f t="shared" si="6"/>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B106" s="11"/>
       <c r="C106" s="12"/>
@@ -5269,13 +5338,13 @@
         <v>116</v>
       </c>
       <c r="F106" s="13">
-        <f t="shared" si="5"/>
-        <v>102</v>
+        <f t="shared" si="6"/>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B107" s="11"/>
       <c r="C107" s="12"/>
@@ -5286,13 +5355,13 @@
         <v>116</v>
       </c>
       <c r="F107" s="13">
-        <f t="shared" si="5"/>
-        <v>103</v>
+        <f t="shared" si="6"/>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B108" s="11"/>
       <c r="C108" s="12"/>
@@ -5303,13 +5372,13 @@
         <v>116</v>
       </c>
       <c r="F108" s="13">
-        <f t="shared" si="5"/>
-        <v>104</v>
+        <f t="shared" si="6"/>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="10" t="s">
-        <v>66</v>
+      <c r="A109" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="B109" s="11"/>
       <c r="C109" s="12"/>
@@ -5320,13 +5389,13 @@
         <v>116</v>
       </c>
       <c r="F109" s="13">
-        <f t="shared" si="5"/>
-        <v>105</v>
+        <f t="shared" si="6"/>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B110" s="11"/>
       <c r="C110" s="12"/>
@@ -5337,13 +5406,13 @@
         <v>116</v>
       </c>
       <c r="F110" s="13">
-        <f t="shared" si="5"/>
-        <v>106</v>
+        <f t="shared" si="6"/>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B111" s="11"/>
       <c r="C111" s="12"/>
@@ -5354,17 +5423,15 @@
         <v>116</v>
       </c>
       <c r="F111" s="13">
-        <f t="shared" si="5"/>
-        <v>107</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>124</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B112" s="11"/>
       <c r="C112" s="12"/>
       <c r="D112" s="12" t="s">
         <v>132</v>
@@ -5373,13 +5440,13 @@
         <v>116</v>
       </c>
       <c r="F112" s="13">
-        <f t="shared" si="5"/>
-        <v>108</v>
+        <f t="shared" si="6"/>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B113" s="11" t="s">
         <v>124</v>
@@ -5392,15 +5459,17 @@
         <v>116</v>
       </c>
       <c r="F113" s="13">
-        <f t="shared" si="5"/>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B114" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="B114" s="11" t="s">
+        <v>124</v>
+      </c>
       <c r="C114" s="12"/>
       <c r="D114" s="12" t="s">
         <v>132</v>
@@ -5409,13 +5478,13 @@
         <v>116</v>
       </c>
       <c r="F114" s="13">
-        <f t="shared" si="5"/>
-        <v>110</v>
+        <f t="shared" si="6"/>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B115" s="11"/>
       <c r="C115" s="12"/>
@@ -5426,38 +5495,47 @@
         <v>116</v>
       </c>
       <c r="F115" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B116" s="11"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E116" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F116" s="13">
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="10" t="s">
+    <row r="117" spans="1:6" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B116" s="11" t="s">
+      <c r="B117" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C116" s="12" t="s">
+      <c r="C117" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D116" s="12" t="s">
+      <c r="D117" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E116" s="11" t="s">
+      <c r="E117" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="F116" s="13">
-        <f t="shared" si="5"/>
+      <c r="F117" s="13">
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="10"/>
-      <c r="B117" s="11"/>
-      <c r="C117" s="12"/>
-      <c r="D117" s="12"/>
-      <c r="E117" s="11"/>
-      <c r="F117" s="13"/>
     </row>
     <row r="118" spans="1:6" s="29" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="30" t="s">
@@ -5470,16 +5548,19 @@
         <v>0</v>
       </c>
       <c r="D118" s="31">
-        <f>COUNTIFS(E51:E117,"Oui")</f>
+        <f>COUNTIFS(E52:E117,"Oui")</f>
         <v>1</v>
       </c>
       <c r="E118" s="32" t="str">
-        <f>IF(COUNTIF(E51:E116,"*Oui*")&lt;&gt;0, "Oui", "Non")</f>
+        <f>IF(COUNTIF(E52:E117,"*Oui*")&lt;&gt;0, "Oui", "Non")</f>
         <v>Oui</v>
       </c>
       <c r="F118" s="33"/>
     </row>
     <row r="119" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="66" t="s">
+        <v>290</v>
+      </c>
       <c r="F119" s="34"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -20132,12 +20213,20 @@
       <c r="F5002" s="34"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="beginsWith" dxfId="95" priority="1" operator="beginsWith" text="Non">
+  <conditionalFormatting sqref="A1:E48 A50:E1048576">
+    <cfRule type="beginsWith" dxfId="39" priority="3" operator="beginsWith" text="Non">
       <formula>LEFT(A1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="2" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="38" priority="4" operator="beginsWith" text="Oui">
       <formula>LEFT(A1,LEN("Oui"))="Oui"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49:E49">
+    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="Non">
+      <formula>LEFT(A49,LEN("Non"))="Non"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="Oui">
+      <formula>LEFT(A49,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20290,18 +20379,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576 E1:E1048576 G1:G1048576">
-    <cfRule type="containsText" dxfId="83" priority="3" operator="containsText" text="Ok">
+    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="Ok">
       <formula>NOT(ISERROR(SEARCH("Ok",C1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="82" priority="4" operator="beginsWith" text="Echec">
+    <cfRule type="beginsWith" dxfId="36" priority="4" operator="beginsWith" text="Echec">
       <formula>LEFT(C1,LEN("Echec"))="Echec"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="81" priority="1" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="2" operator="containsText" text="Oui">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Oui">
       <formula>NOT(ISERROR(SEARCH("Oui",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20320,7 +20409,7 @@
   </sheetPr>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
@@ -21098,82 +21187,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1:L21 L25:L1048576 F25:F1048576 F1:F22">
-    <cfRule type="beginsWith" dxfId="63" priority="25" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="33" priority="25" operator="beginsWith" text="Non">
       <formula>LEFT(F1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="62" priority="26" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="32" priority="26" operator="beginsWith" text="Oui">
       <formula>LEFT(F1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M21 M25:M1048576">
-    <cfRule type="beginsWith" dxfId="61" priority="23" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="31" priority="23" operator="beginsWith" text="Oui">
       <formula>LEFT(M1,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="24" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="30" priority="24" operator="beginsWith" text="Non">
       <formula>LEFT(M1,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="beginsWith" dxfId="59" priority="21" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="29" priority="21" operator="beginsWith" text="Non">
       <formula>LEFT(F19,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="22" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="28" priority="22" operator="beginsWith" text="Oui">
       <formula>LEFT(F19,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="beginsWith" dxfId="57" priority="19" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="27" priority="19" operator="beginsWith" text="Non">
       <formula>LEFT(L19,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="20" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="26" priority="20" operator="beginsWith" text="Oui">
       <formula>LEFT(L19,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19">
-    <cfRule type="beginsWith" dxfId="55" priority="17" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="25" priority="17" operator="beginsWith" text="Oui">
       <formula>LEFT(M19,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="18" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="24" priority="18" operator="beginsWith" text="Non">
       <formula>LEFT(M19,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="beginsWith" dxfId="53" priority="15" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="23" priority="15" operator="beginsWith" text="Non">
       <formula>LEFT(F21,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="16" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="22" priority="16" operator="beginsWith" text="Oui">
       <formula>LEFT(F21,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="beginsWith" dxfId="51" priority="13" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="21" priority="13" operator="beginsWith" text="Non">
       <formula>LEFT(L21,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="14" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="20" priority="14" operator="beginsWith" text="Oui">
       <formula>LEFT(L21,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="beginsWith" dxfId="49" priority="11" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="19" priority="11" operator="beginsWith" text="Oui">
       <formula>LEFT(M21,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="12" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="18" priority="12" operator="beginsWith" text="Non">
       <formula>LEFT(M21,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="beginsWith" dxfId="47" priority="3" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="17" priority="3" operator="beginsWith" text="Non">
       <formula>LEFT(F20,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="4" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="16" priority="4" operator="beginsWith" text="Oui">
       <formula>LEFT(F20,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="beginsWith" dxfId="45" priority="1" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="15" priority="1" operator="beginsWith" text="Non">
       <formula>LEFT(F22,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="2" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="14" priority="2" operator="beginsWith" text="Oui">
       <formula>LEFT(F22,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21298,42 +21387,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E3 J1:J3">
-    <cfRule type="beginsWith" dxfId="25" priority="9" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="13" priority="9" operator="beginsWith" text="Non">
       <formula>LEFT(E1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="10" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="12" priority="10" operator="beginsWith" text="Oui">
       <formula>LEFT(E1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K3">
-    <cfRule type="beginsWith" dxfId="23" priority="7" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="11" priority="7" operator="beginsWith" text="Oui">
       <formula>LEFT(K1,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="8" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="10" priority="8" operator="beginsWith" text="Non">
       <formula>LEFT(K1,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="beginsWith" dxfId="21" priority="1" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="9" priority="1" operator="beginsWith" text="Oui">
       <formula>LEFT(K1,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="2" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="8" priority="2" operator="beginsWith" text="Non">
       <formula>LEFT(K1,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="beginsWith" dxfId="19" priority="5" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="7" priority="5" operator="beginsWith" text="Non">
       <formula>LEFT(E1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="6" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="6" priority="6" operator="beginsWith" text="Oui">
       <formula>LEFT(E1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="beginsWith" dxfId="17" priority="3" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="5" priority="3" operator="beginsWith" text="Non">
       <formula>LEFT(J1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="4" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="4" priority="4" operator="beginsWith" text="Oui">
       <formula>LEFT(J1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ajout du contrôle pour le test M29
</commit_message>
<xml_diff>
--- a/Documentation/Developpement/Tableau_des_tests_effectues.xlsx
+++ b/Documentation/Developpement/Tableau_des_tests_effectues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tests auto" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="307">
   <si>
     <t>Nom</t>
   </si>
@@ -933,6 +933,15 @@
   </si>
   <si>
     <t>"La balise ArchivalAgreement ne doit pas être contenue dans la data"</t>
+  </si>
+  <si>
+    <t>ArchivalAgreement</t>
+  </si>
+  <si>
+    <t>ArchivetTransfer/Contains</t>
+  </si>
+  <si>
+    <t>ArchivetTransfer/Archive</t>
   </si>
 </sst>
 </file>
@@ -1431,539 +1440,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="108">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2171,6 +1648,106 @@
         </vertical>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2624,6 +2201,206 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3000,6 +2777,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3125,6 +2942,174 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3136,78 +3121,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:F5008" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:F5008" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90">
   <tableColumns count="6">
-    <tableColumn id="1" name="Nom" dataDxfId="105"/>
-    <tableColumn id="2" name="Role" dataDxfId="104"/>
-    <tableColumn id="3" name="Resultat attendu" dataDxfId="103"/>
-    <tableColumn id="4" name="Resultat obtenu si echec" dataDxfId="102"/>
-    <tableColumn id="5" name="Modification a prevoir" dataDxfId="101"/>
-    <tableColumn id="6" name="Numéro d'ordre" dataDxfId="100"/>
+    <tableColumn id="1" name="Nom" dataDxfId="89"/>
+    <tableColumn id="2" name="Role" dataDxfId="88"/>
+    <tableColumn id="3" name="Resultat attendu" dataDxfId="87"/>
+    <tableColumn id="4" name="Resultat obtenu si echec" dataDxfId="86"/>
+    <tableColumn id="5" name="Modification a prevoir" dataDxfId="85"/>
+    <tableColumn id="6" name="Numéro d'ordre" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
   <tableColumns count="11">
-    <tableColumn id="1" name="Profil testé" dataDxfId="94"/>
-    <tableColumn id="2" name="Nom tâche" dataDxfId="93"/>
-    <tableColumn id="3" name="Résultat test1" dataDxfId="92"/>
-    <tableColumn id="4" name="Si echec, stopper ici et écrire erreur test1" dataDxfId="91"/>
-    <tableColumn id="5" name="Résultat test2" dataDxfId="90"/>
-    <tableColumn id="6" name="Si echec, stopper ici et écrire erreur test2" dataDxfId="89"/>
-    <tableColumn id="7" name="Résultat test3" dataDxfId="88"/>
-    <tableColumn id="8" name="Si echec, stopper ici et écrire erreur test3" dataDxfId="87"/>
-    <tableColumn id="9" name="A revoir ?" dataDxfId="86"/>
-    <tableColumn id="10" name="Test à modifier" dataDxfId="85"/>
-    <tableColumn id="11" name="Phrase d'explication à mettre pour l'erreur" dataDxfId="84"/>
+    <tableColumn id="1" name="Profil testé" dataDxfId="74"/>
+    <tableColumn id="2" name="Nom tâche" dataDxfId="73"/>
+    <tableColumn id="3" name="Résultat test1" dataDxfId="72"/>
+    <tableColumn id="4" name="Si echec, stopper ici et écrire erreur test1" dataDxfId="71"/>
+    <tableColumn id="5" name="Résultat test2" dataDxfId="70"/>
+    <tableColumn id="6" name="Si echec, stopper ici et écrire erreur test2" dataDxfId="69"/>
+    <tableColumn id="7" name="Résultat test3" dataDxfId="68"/>
+    <tableColumn id="8" name="Si echec, stopper ici et écrire erreur test3" dataDxfId="67"/>
+    <tableColumn id="9" name="A revoir ?" dataDxfId="66"/>
+    <tableColumn id="10" name="Test à modifier" dataDxfId="65"/>
+    <tableColumn id="11" name="Phrase d'explication à mettre pour l'erreur" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:N1048576" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80">
-  <sortState ref="A2:N29">
-    <sortCondition ref="A2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:N1048576" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40">
+  <sortState ref="A2:N30">
+    <sortCondition ref="G1"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Balise strictement obligatoire" dataDxfId="79"/>
-    <tableColumn id="2" name="Nom en français" dataDxfId="78"/>
-    <tableColumn id="3" name="Version du SEDA" dataDxfId="77"/>
-    <tableColumn id="13" name="Chemin" dataDxfId="76"/>
-    <tableColumn id="4" name="Source auto, métier ou database" dataDxfId="75"/>
-    <tableColumn id="5" name="Créée lors de test ?" dataDxfId="74"/>
-    <tableColumn id="6" name="Balise falcultative" dataDxfId="73"/>
-    <tableColumn id="7" name="Nom en français2" dataDxfId="72"/>
-    <tableColumn id="8" name="Version" dataDxfId="71"/>
-    <tableColumn id="9" name="Chemin2" dataDxfId="70"/>
-    <tableColumn id="14" name="Source auto, métier ou database2" dataDxfId="69"/>
-    <tableColumn id="10" name="Quand obligatoire, créée lors de test ?" dataDxfId="68"/>
-    <tableColumn id="11" name="Quand falcultative, créée lors de test ?" dataDxfId="67"/>
-    <tableColumn id="12" name="Quand non-demandé, créée lors de test ?" dataDxfId="66"/>
+    <tableColumn id="1" name="Balise strictement obligatoire" dataDxfId="39"/>
+    <tableColumn id="2" name="Nom en français" dataDxfId="38"/>
+    <tableColumn id="3" name="Version du SEDA" dataDxfId="37"/>
+    <tableColumn id="13" name="Chemin" dataDxfId="36"/>
+    <tableColumn id="4" name="Source auto, métier ou database" dataDxfId="35"/>
+    <tableColumn id="5" name="Créée lors de test ?" dataDxfId="34"/>
+    <tableColumn id="6" name="Balise falcultative" dataDxfId="33"/>
+    <tableColumn id="7" name="Nom en français2" dataDxfId="32"/>
+    <tableColumn id="8" name="Version" dataDxfId="31"/>
+    <tableColumn id="9" name="Chemin2" dataDxfId="30"/>
+    <tableColumn id="14" name="Source auto, métier ou database2" dataDxfId="29"/>
+    <tableColumn id="10" name="Quand obligatoire, créée lors de test ?" dataDxfId="28"/>
+    <tableColumn id="11" name="Quand falcultative, créée lors de test ?" dataDxfId="27"/>
+    <tableColumn id="12" name="Quand non-demandé, créée lors de test ?" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A1:L1048576" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A1:L1048576" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <tableColumns count="12">
-    <tableColumn id="1" name="Attribut strictement obligatoire en v1.0" dataDxfId="61"/>
-    <tableColumn id="2" name="Nom en français" dataDxfId="60"/>
-    <tableColumn id="3" name="Version du SEDA" dataDxfId="59"/>
-    <tableColumn id="4" name="Chemin" dataDxfId="58"/>
-    <tableColumn id="5" name="Créée lors de test ?" dataDxfId="57"/>
-    <tableColumn id="6" name="Attribut falcultatif" dataDxfId="56"/>
-    <tableColumn id="7" name="Nom en français2" dataDxfId="55"/>
-    <tableColumn id="8" name="Version" dataDxfId="54"/>
-    <tableColumn id="9" name="Chemin2" dataDxfId="53"/>
-    <tableColumn id="10" name="Quand obligatoire, créée lors de test ?" dataDxfId="52"/>
-    <tableColumn id="11" name="Quand falcultatif, créée lors de test ?" dataDxfId="51"/>
-    <tableColumn id="12" name="Quand non-demandé, créé lors de test ?" dataDxfId="50"/>
+    <tableColumn id="1" name="Attribut strictement obligatoire en v1.0" dataDxfId="11"/>
+    <tableColumn id="2" name="Nom en français" dataDxfId="10"/>
+    <tableColumn id="3" name="Version du SEDA" dataDxfId="9"/>
+    <tableColumn id="4" name="Chemin" dataDxfId="8"/>
+    <tableColumn id="5" name="Créée lors de test ?" dataDxfId="7"/>
+    <tableColumn id="6" name="Attribut falcultatif" dataDxfId="6"/>
+    <tableColumn id="7" name="Nom en français2" dataDxfId="5"/>
+    <tableColumn id="8" name="Version" dataDxfId="4"/>
+    <tableColumn id="9" name="Chemin2" dataDxfId="3"/>
+    <tableColumn id="10" name="Quand obligatoire, créée lors de test ?" dataDxfId="2"/>
+    <tableColumn id="11" name="Quand falcultatif, créée lors de test ?" dataDxfId="1"/>
+    <tableColumn id="12" name="Quand non-demandé, créé lors de test ?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3505,7 +3490,7 @@
   </sheetPr>
   <dimension ref="A1:F5008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
@@ -20491,58 +20476,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A56:E1048576 E52:E54 A1:E49">
-    <cfRule type="beginsWith" dxfId="49" priority="13" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="107" priority="13" operator="beginsWith" text="Non">
       <formula>LEFT(A1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="14" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="106" priority="14" operator="beginsWith" text="Oui">
       <formula>LEFT(A1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:E50">
-    <cfRule type="beginsWith" dxfId="47" priority="11" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="105" priority="11" operator="beginsWith" text="Non">
       <formula>LEFT(A50,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="12" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="104" priority="12" operator="beginsWith" text="Oui">
       <formula>LEFT(A50,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:E51 A53:B55 D52:D54">
-    <cfRule type="beginsWith" dxfId="45" priority="9" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="103" priority="9" operator="beginsWith" text="Non">
       <formula>LEFT(A51,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="10" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="102" priority="10" operator="beginsWith" text="Oui">
       <formula>LEFT(A51,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:C52">
-    <cfRule type="beginsWith" dxfId="43" priority="7" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="101" priority="7" operator="beginsWith" text="Non">
       <formula>LEFT(A52,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="8" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="100" priority="8" operator="beginsWith" text="Oui">
       <formula>LEFT(A52,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="beginsWith" dxfId="41" priority="5" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="99" priority="5" operator="beginsWith" text="Non">
       <formula>LEFT(C53,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="6" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="98" priority="6" operator="beginsWith" text="Oui">
       <formula>LEFT(C53,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="beginsWith" dxfId="39" priority="3" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="97" priority="3" operator="beginsWith" text="Non">
       <formula>LEFT(C54,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="4" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="96" priority="4" operator="beginsWith" text="Oui">
       <formula>LEFT(C54,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:E55">
-    <cfRule type="beginsWith" dxfId="37" priority="1" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="95" priority="1" operator="beginsWith" text="Non">
       <formula>LEFT(D55,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="2" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="94" priority="2" operator="beginsWith" text="Oui">
       <formula>LEFT(D55,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20696,18 +20681,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576 E1:E1048576 G1:G1048576">
-    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="Ok">
+    <cfRule type="containsText" dxfId="83" priority="3" operator="containsText" text="Ok">
       <formula>NOT(ISERROR(SEARCH("Ok",C1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="4" operator="beginsWith" text="Echec">
+    <cfRule type="beginsWith" dxfId="82" priority="4" operator="beginsWith" text="Echec">
       <formula>LEFT(C1,LEN("Echec"))="Echec"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="81" priority="1" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Oui">
+    <cfRule type="containsText" dxfId="80" priority="2" operator="containsText" text="Oui">
       <formula>NOT(ISERROR(SEARCH("Oui",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20726,9 +20711,9 @@
   </sheetPr>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20796,57 +20781,53 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="B2" s="60"/>
       <c r="C2" s="60" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D2" s="60" t="s">
-        <v>244</v>
-      </c>
-      <c r="E2" s="60" t="s">
-        <v>266</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="E2" s="60"/>
       <c r="F2" s="55"/>
       <c r="G2" s="59" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="H2" s="60"/>
       <c r="I2" s="60" t="s">
         <v>254</v>
       </c>
       <c r="J2" s="60" t="s">
-        <v>278</v>
-      </c>
-      <c r="K2" s="60" t="s">
-        <v>269</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="K2" s="60"/>
       <c r="L2" s="60"/>
       <c r="M2" s="60"/>
       <c r="N2" s="55"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>222</v>
+        <v>255</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="I3" s="47" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J3" s="47" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="K3" s="60" t="s">
         <v>269</v>
@@ -20854,25 +20835,25 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>221</v>
+        <v>249</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="I4" s="47" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="J4" s="47" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="K4" s="60" t="s">
         <v>269</v>
@@ -20880,187 +20861,204 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>285</v>
+        <v>241</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>256</v>
       </c>
       <c r="D5" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>265</v>
+      </c>
+      <c r="I5" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="J5" s="47" t="s">
         <v>244</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>266</v>
-      </c>
-      <c r="G5" s="46" t="s">
-        <v>276</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="J5" s="47" t="s">
-        <v>280</v>
       </c>
       <c r="K5" s="60" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>222</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="I6" s="47" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J6" s="47" t="s">
         <v>215</v>
       </c>
       <c r="K6" s="60" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>223</v>
+        <v>246</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>255</v>
       </c>
       <c r="E7" s="47" t="s">
         <v>269</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>230</v>
+        <v>273</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
+      </c>
+      <c r="J7" s="47" t="s">
+        <v>264</v>
       </c>
       <c r="K7" s="60" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>221</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>254</v>
       </c>
+      <c r="D8" s="47" t="s">
+        <v>255</v>
+      </c>
       <c r="E8" s="47" t="s">
         <v>269</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>225</v>
+        <v>273</v>
       </c>
       <c r="I8" s="47" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="J8" s="47" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="K8" s="60" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
-        <v>287</v>
+        <v>241</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>242</v>
-      </c>
-      <c r="K9" s="60"/>
+        <v>243</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="I9" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="K9" s="60" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D10" s="47" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E10" s="47" t="s">
         <v>266</v>
       </c>
       <c r="G10" s="46" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>257</v>
       </c>
+      <c r="J10" s="47" t="s">
+        <v>249</v>
+      </c>
       <c r="K10" s="60" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="E11" s="47" t="s">
         <v>269</v>
       </c>
       <c r="G11" s="46" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="I11" s="47" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J11" s="47" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="K11" s="60" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
       <c r="C12" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="I12" s="47" t="s">
         <v>256</v>
       </c>
-      <c r="D12" s="47" t="s">
-        <v>242</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>269</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>276</v>
-      </c>
-      <c r="I12" s="47" t="s">
-        <v>254</v>
-      </c>
       <c r="J12" s="47" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="K12" s="47" t="s">
         <v>269</v>
@@ -21068,36 +21066,48 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>288</v>
+        <v>241</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>256</v>
       </c>
       <c r="D13" s="47" t="s">
-        <v>272</v>
+        <v>242</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>232</v>
+      </c>
+      <c r="I13" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="J13" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="K13" s="47" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>215</v>
+        <v>284</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>256</v>
       </c>
       <c r="D14" s="47" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="E14" s="47" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G14" s="46" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="I14" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J14" s="47" t="s">
         <v>215</v>
@@ -21106,79 +21116,82 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>254</v>
       </c>
-      <c r="D15" s="47" t="s">
-        <v>243</v>
-      </c>
       <c r="E15" s="47" t="s">
         <v>269</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="I15" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
+      </c>
+      <c r="J15" s="47" t="s">
+        <v>263</v>
       </c>
       <c r="K15" s="47" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>245</v>
+        <v>222</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>214</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>256</v>
       </c>
       <c r="D16" s="47" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E16" s="47" t="s">
         <v>269</v>
       </c>
       <c r="G16" s="46" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="I16" s="47" t="s">
         <v>256</v>
       </c>
       <c r="J16" s="47" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="K16" s="60" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D17" s="47" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
       <c r="E17" s="47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G17" s="46" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="I17" s="47" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J17" s="47" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="K17" s="60" t="s">
         <v>269</v>
@@ -21186,25 +21199,25 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>245</v>
+        <v>286</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="47" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E18" s="47" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="I18" s="47" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J18" s="47" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
       <c r="K18" s="60" t="s">
         <v>269</v>
@@ -21212,25 +21225,25 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D19" s="47" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="E19" s="47" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G19" s="46" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="I19" s="47" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="J19" s="47" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="K19" s="60" t="s">
         <v>269</v>
@@ -21238,25 +21251,25 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
-        <v>246</v>
+        <v>285</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D20" s="47" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="E20" s="47" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G20" s="46" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="I20" s="47" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="J20" s="47" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="K20" s="60" t="s">
         <v>269</v>
@@ -21264,33 +21277,33 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
-        <v>241</v>
+        <v>215</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>215</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D21" s="47" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E21" s="47" t="s">
         <v>269</v>
       </c>
       <c r="G21" s="46" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I21" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="J21" s="47" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="K21" s="60" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C22" s="47" t="s">
         <v>256</v>
@@ -21302,13 +21315,13 @@
         <v>269</v>
       </c>
       <c r="G22" s="46" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="I22" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J22" s="47" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="K22" s="60" t="s">
         <v>269</v>
@@ -21316,28 +21329,25 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C23" s="47" t="s">
         <v>257</v>
       </c>
       <c r="D23" s="47" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E23" s="47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G23" s="46" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I23" s="47" t="s">
         <v>257</v>
       </c>
-      <c r="J23" s="47" t="s">
-        <v>215</v>
-      </c>
       <c r="K23" s="60" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -21366,19 +21376,22 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
-        <v>241</v>
+        <v>215</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>215</v>
       </c>
       <c r="C25" s="47" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D25" s="47" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="E25" s="47" t="s">
         <v>269</v>
       </c>
       <c r="G25" s="46" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="I25" s="47" t="s">
         <v>257</v>
@@ -21387,64 +21400,61 @@
         <v>215</v>
       </c>
       <c r="K25" s="60" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E26" s="47" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="G26" s="46" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I26" s="47" t="s">
         <v>257</v>
       </c>
-      <c r="J26" s="47" t="s">
-        <v>249</v>
-      </c>
       <c r="K26" s="60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>241</v>
+        <v>283</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>256</v>
       </c>
       <c r="D27" s="47" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="E27" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="G27" s="46" t="s">
+        <v>279</v>
+      </c>
+      <c r="I27" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="J27" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="K27" s="60" t="s">
         <v>269</v>
-      </c>
-      <c r="G27" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="I27" s="47" t="s">
-        <v>257</v>
-      </c>
-      <c r="J27" s="47" t="s">
-        <v>248</v>
-      </c>
-      <c r="K27" s="60" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D28" s="47" t="s">
         <v>244</v>
@@ -21453,133 +21463,128 @@
         <v>266</v>
       </c>
       <c r="G28" s="46" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
       <c r="I28" s="47" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="J28" s="47" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="K28" s="47" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D29" s="47" t="s">
-        <v>244</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>266</v>
-      </c>
-      <c r="G29" s="46" t="s">
-        <v>279</v>
-      </c>
-      <c r="I29" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="G29" s="59" t="s">
+        <v>304</v>
+      </c>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60" t="s">
         <v>256</v>
       </c>
-      <c r="J29" s="47" t="s">
-        <v>277</v>
-      </c>
-      <c r="K29" s="47" t="s">
-        <v>269</v>
+      <c r="J29" s="60" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D30" s="47" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1:L21 L25:L1048576 F25:F1048576 F1:F22">
-    <cfRule type="beginsWith" dxfId="31" priority="25" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="63" priority="25" operator="beginsWith" text="Non">
       <formula>LEFT(F1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="26" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="62" priority="26" operator="beginsWith" text="Oui">
       <formula>LEFT(F1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M21 M25:M1048576">
-    <cfRule type="beginsWith" dxfId="29" priority="23" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="61" priority="23" operator="beginsWith" text="Oui">
       <formula>LEFT(M1,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="24" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="60" priority="24" operator="beginsWith" text="Non">
       <formula>LEFT(M1,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="beginsWith" dxfId="27" priority="21" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="59" priority="21" operator="beginsWith" text="Non">
       <formula>LEFT(F19,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="22" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="58" priority="22" operator="beginsWith" text="Oui">
       <formula>LEFT(F19,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="beginsWith" dxfId="25" priority="19" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="57" priority="19" operator="beginsWith" text="Non">
       <formula>LEFT(L19,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="20" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="56" priority="20" operator="beginsWith" text="Oui">
       <formula>LEFT(L19,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19">
-    <cfRule type="beginsWith" dxfId="23" priority="17" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="55" priority="17" operator="beginsWith" text="Oui">
       <formula>LEFT(M19,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="18" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="54" priority="18" operator="beginsWith" text="Non">
       <formula>LEFT(M19,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="beginsWith" dxfId="21" priority="15" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="53" priority="15" operator="beginsWith" text="Non">
       <formula>LEFT(F21,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="16" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="52" priority="16" operator="beginsWith" text="Oui">
       <formula>LEFT(F21,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="beginsWith" dxfId="19" priority="13" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="51" priority="13" operator="beginsWith" text="Non">
       <formula>LEFT(L21,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="14" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="50" priority="14" operator="beginsWith" text="Oui">
       <formula>LEFT(L21,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="beginsWith" dxfId="17" priority="11" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="49" priority="11" operator="beginsWith" text="Oui">
       <formula>LEFT(M21,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="12" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="48" priority="12" operator="beginsWith" text="Non">
       <formula>LEFT(M21,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="beginsWith" dxfId="15" priority="3" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="47" priority="3" operator="beginsWith" text="Non">
       <formula>LEFT(F20,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="4" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="46" priority="4" operator="beginsWith" text="Oui">
       <formula>LEFT(F20,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="beginsWith" dxfId="13" priority="1" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="45" priority="1" operator="beginsWith" text="Non">
       <formula>LEFT(F22,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="2" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="44" priority="2" operator="beginsWith" text="Oui">
       <formula>LEFT(F22,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21704,42 +21709,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E3 J1:J3">
-    <cfRule type="beginsWith" dxfId="11" priority="9" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="25" priority="9" operator="beginsWith" text="Non">
       <formula>LEFT(E1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="10" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="24" priority="10" operator="beginsWith" text="Oui">
       <formula>LEFT(E1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K3">
-    <cfRule type="beginsWith" dxfId="9" priority="7" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="23" priority="7" operator="beginsWith" text="Oui">
       <formula>LEFT(K1,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="22" priority="8" operator="beginsWith" text="Non">
       <formula>LEFT(K1,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="beginsWith" dxfId="7" priority="1" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="21" priority="1" operator="beginsWith" text="Oui">
       <formula>LEFT(K1,LEN("Oui"))="Oui"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="2" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="20" priority="2" operator="beginsWith" text="Non">
       <formula>LEFT(K1,LEN("Non"))="Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="beginsWith" dxfId="5" priority="5" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="19" priority="5" operator="beginsWith" text="Non">
       <formula>LEFT(E1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="6" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="18" priority="6" operator="beginsWith" text="Oui">
       <formula>LEFT(E1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="beginsWith" dxfId="3" priority="3" operator="beginsWith" text="Non">
+    <cfRule type="beginsWith" dxfId="17" priority="3" operator="beginsWith" text="Non">
       <formula>LEFT(J1,LEN("Non"))="Non"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="4" operator="beginsWith" text="Oui">
+    <cfRule type="beginsWith" dxfId="16" priority="4" operator="beginsWith" text="Oui">
       <formula>LEFT(J1,LEN("Oui"))="Oui"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>